<commit_message>
minor changes to VaR xls
</commit_message>
<xml_diff>
--- a/M2/VaR.xlsx
+++ b/M2/VaR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="11520" windowHeight="8100" tabRatio="560"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="560"/>
   </bookViews>
   <sheets>
     <sheet name="Historic Data" sheetId="4" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>Breach_t-1</t>
   </si>
   <si>
-    <t>Conditional Probability</t>
-  </si>
-  <si>
     <t>r</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>% Breaches</t>
+  </si>
+  <si>
+    <t>Conditional Probability (Baye's Theorem)</t>
   </si>
 </sst>
 </file>
@@ -6369,11 +6369,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2067079944"/>
-        <c:axId val="2067082216"/>
+        <c:axId val="2091701960"/>
+        <c:axId val="2091703864"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2067079944"/>
+        <c:axId val="2091701960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6383,14 +6383,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067082216"/>
+        <c:crossAx val="2091703864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2067082216"/>
+        <c:axId val="2091703864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6401,7 +6401,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067079944"/>
+        <c:crossAx val="2091701960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12532,11 +12532,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2067119144"/>
-        <c:axId val="2067122152"/>
+        <c:axId val="2091777336"/>
+        <c:axId val="2091780360"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2067119144"/>
+        <c:axId val="2091777336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12546,14 +12546,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067122152"/>
+        <c:crossAx val="2091780360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2067122152"/>
+        <c:axId val="2091780360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12564,7 +12564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067119144"/>
+        <c:crossAx val="2091777336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13026,11 +13026,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2067149176"/>
-        <c:axId val="2067154328"/>
+        <c:axId val="2091807512"/>
+        <c:axId val="2091812696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2067149176"/>
+        <c:axId val="2091807512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13043,7 +13043,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067154328"/>
+        <c:crossAx val="2091812696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13051,7 +13051,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2067154328"/>
+        <c:axId val="2091812696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13065,7 +13065,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067149176"/>
+        <c:crossAx val="2091807512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25083,11 +25083,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2066619512"/>
-        <c:axId val="2067171992"/>
+        <c:axId val="2091849560"/>
+        <c:axId val="2091852824"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2066619512"/>
+        <c:axId val="2091849560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25105,14 +25105,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067171992"/>
+        <c:crossAx val="2091852824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2067171992"/>
+        <c:axId val="2091852824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25123,7 +25123,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066619512"/>
+        <c:crossAx val="2091849560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25640,6 +25640,59 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>517525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Oval 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16583025" y="3686175"/>
+          <a:ext cx="238125" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -25955,10 +26008,10 @@
         <v>12</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -26044,7 +26097,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>7</v>
@@ -26056,7 +26109,7 @@
         <v>9</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>13</v>
@@ -26065,7 +26118,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" s="11"/>
     </row>
@@ -65371,7 +65424,7 @@
         <v>-2.149633553293917E-2</v>
       </c>
       <c r="H991">
-        <f t="shared" ref="H991:H1054" si="123">IF(G991="", "",IF(G991&lt;F991,1, 0))</f>
+        <f t="shared" ref="H991:H1018" si="123">IF(G991="", "",IF(G991&lt;F991,1, 0))</f>
         <v>0</v>
       </c>
       <c r="I991">

</xml_diff>